<commit_message>
updated ctrlpy and examples for max deductible allocation method
</commit_message>
<xml_diff>
--- a/ftest/fm28/Worked example policy calculation_Max deductibles_Layers_ILallocated.xlsx
+++ b/ftest/fm28/Worked example policy calculation_Max deductibles_Layers_ILallocated.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm28\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\joh\dev\ktest\ftest\fm28\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{498EB04D-6CFB-426D-BFAA-11512BED2F01}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96453B4-3020-4C25-B864-4564695237FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worked examples" sheetId="10" r:id="rId1"/>
     <sheet name="Oasis Implementation" sheetId="8" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="137">
   <si>
     <t>Limit</t>
   </si>
@@ -437,12 +448,6 @@
     <t>Loss by policy layer</t>
   </si>
   <si>
-    <t>Layer 1 Loss</t>
-  </si>
-  <si>
-    <t>Layer 2 Loss</t>
-  </si>
-  <si>
     <t>Xref</t>
   </si>
   <si>
@@ -453,6 +458,33 @@
   </si>
   <si>
     <t>layer_id</t>
+  </si>
+  <si>
+    <t>Underlimit</t>
+  </si>
+  <si>
+    <t>Loss allocation underlimit</t>
+  </si>
+  <si>
+    <t>Loss allocation prior level</t>
+  </si>
+  <si>
+    <t>Layer 1 Loss  (Prior Level - updated August 2021)</t>
+  </si>
+  <si>
+    <t>Layer 1 Loss (Prior Level)</t>
+  </si>
+  <si>
+    <t>Layer 2 Loss (Prior Level)</t>
+  </si>
+  <si>
+    <t>Layer 2 Loss  (Prior Level - updated August 2021)</t>
+  </si>
+  <si>
+    <t>Loss adjustment</t>
+  </si>
+  <si>
+    <t>Weighted allocation new method</t>
   </si>
 </sst>
 </file>
@@ -464,7 +496,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -572,6 +604,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -772,7 +817,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -917,9 +962,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -963,14 +1005,38 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1384,16 +1450,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="43.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
@@ -1565,18 +1631,18 @@
       <c r="B10" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="86">
+      <c r="C10" s="87">
         <v>0.05</v>
       </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86">
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="87"/>
+      <c r="G10" s="87">
         <v>0.05</v>
       </c>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="87"/>
+      <c r="J10" s="87"/>
       <c r="K10" s="36"/>
       <c r="L10" s="43"/>
     </row>
@@ -1643,14 +1709,14 @@
         <v>115</v>
       </c>
       <c r="B14" s="39"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
       <c r="K14" s="36"/>
       <c r="L14" s="48"/>
     </row>
@@ -1661,14 +1727,14 @@
       <c r="B15" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
       <c r="K15" s="36"/>
       <c r="L15" s="48">
         <v>0</v>
@@ -1909,35 +1975,35 @@
         <v>106</v>
       </c>
       <c r="B26" s="39"/>
-      <c r="C26" s="71">
+      <c r="C26" s="70">
         <f>C25/SUM($C$25:$F$25)</f>
         <v>0.8857395925597874</v>
       </c>
-      <c r="D26" s="71">
+      <c r="D26" s="70">
         <f>D25/SUM($C$25:$F$25)</f>
         <v>8.8573959255978746E-2</v>
       </c>
-      <c r="E26" s="71">
+      <c r="E26" s="70">
         <f>E25/SUM($C$25:$F$25)</f>
         <v>2.2143489813994686E-2</v>
       </c>
-      <c r="F26" s="71">
+      <c r="F26" s="70">
         <f>F25/SUM($C$25:$F$25)</f>
         <v>3.5429583702391498E-3</v>
       </c>
-      <c r="G26" s="71">
+      <c r="G26" s="70">
         <f>G25/SUM($G$25:$J$25)</f>
         <v>1</v>
       </c>
-      <c r="H26" s="71">
+      <c r="H26" s="70">
         <f>H25/SUM($G$25:$J$25)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="71">
+      <c r="I26" s="70">
         <f>I25/SUM($G$25:$J$25)</f>
         <v>0</v>
       </c>
-      <c r="J26" s="71">
+      <c r="J26" s="70">
         <f>J25/SUM($G$25:$J$25)</f>
         <v>0</v>
       </c>
@@ -1945,20 +2011,20 @@
       <c r="L26" s="58"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="73"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="76"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
+      <c r="H27" s="73"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="73"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="75"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="38" t="s">
@@ -1967,20 +2033,20 @@
       <c r="B28" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="87">
+      <c r="C28" s="88">
         <f>SUM(C9:F9)*C10</f>
         <v>58500</v>
       </c>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87">
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="88">
         <f>SUM(G9:J9)*G10</f>
         <v>58500</v>
       </c>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="87"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="88"/>
+      <c r="J28" s="88"/>
       <c r="K28" s="57"/>
       <c r="L28" s="58"/>
     </row>
@@ -1991,20 +2057,20 @@
       <c r="B29" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="85">
+      <c r="C29" s="89">
         <f>SUM(C25:F25)</f>
         <v>112900</v>
       </c>
-      <c r="D29" s="85"/>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="85">
+      <c r="D29" s="89"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89">
         <f>SUM(G25:J25)</f>
         <v>10000</v>
       </c>
-      <c r="H29" s="85"/>
-      <c r="I29" s="85"/>
-      <c r="J29" s="85"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="89"/>
+      <c r="J29" s="89"/>
       <c r="K29" s="56"/>
       <c r="L29" s="42"/>
     </row>
@@ -2015,20 +2081,20 @@
       <c r="B30" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="85">
+      <c r="C30" s="89">
         <f>MIN(C29,C28)</f>
         <v>58500</v>
       </c>
-      <c r="D30" s="85"/>
-      <c r="E30" s="85"/>
-      <c r="F30" s="85"/>
-      <c r="G30" s="85">
+      <c r="D30" s="89"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89">
         <f>MIN(G29,G28)</f>
         <v>10000</v>
       </c>
-      <c r="H30" s="85"/>
-      <c r="I30" s="85"/>
-      <c r="J30" s="85"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
       <c r="K30" s="59"/>
       <c r="L30" s="60">
         <f>SUM(C30:J30)</f>
@@ -2043,20 +2109,20 @@
       <c r="B31" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="85">
+      <c r="C31" s="89">
         <f>C29-C30</f>
         <v>54400</v>
       </c>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85">
+      <c r="D31" s="89"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="89">
         <f>G29-G30</f>
         <v>0</v>
       </c>
-      <c r="H31" s="85"/>
-      <c r="I31" s="85"/>
-      <c r="J31" s="85"/>
+      <c r="H31" s="89"/>
+      <c r="I31" s="89"/>
+      <c r="J31" s="89"/>
       <c r="K31" s="59"/>
       <c r="L31" s="60">
         <f>SUM(C31:J31)</f>
@@ -2066,489 +2132,694 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="38" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="B32" s="39"/>
-      <c r="C32" s="84">
-        <f>C31/SUM($C$31:$J$31)</f>
-        <v>1</v>
-      </c>
-      <c r="D32" s="84"/>
-      <c r="E32" s="84"/>
-      <c r="F32" s="84"/>
-      <c r="G32" s="84">
-        <f>G31/SUM($C$31:$J$31)</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="84"/>
-      <c r="I32" s="84"/>
-      <c r="J32" s="84"/>
+      <c r="C32" s="89">
+        <f>C30</f>
+        <v>58500</v>
+      </c>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89">
+        <f>G30</f>
+        <v>10000</v>
+      </c>
+      <c r="H32" s="89"/>
+      <c r="I32" s="89"/>
+      <c r="J32" s="89"/>
       <c r="K32" s="59"/>
       <c r="L32" s="60"/>
       <c r="M32" s="61"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" s="73"/>
-      <c r="C33" s="78"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="78"/>
-      <c r="G33" s="78"/>
-      <c r="H33" s="78"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="78"/>
-      <c r="K33" s="79"/>
-      <c r="L33" s="80"/>
+      <c r="A33" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="39"/>
+      <c r="C33" s="90">
+        <f>C31/SUM($C$31:$J$31)</f>
+        <v>1</v>
+      </c>
+      <c r="D33" s="90"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90">
+        <f>G31/SUM($C$31:$J$31)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="90"/>
+      <c r="I33" s="90"/>
+      <c r="J33" s="90"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="60"/>
       <c r="M33" s="61"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B34" s="39"/>
+      <c r="C34" s="90">
+        <f>C32/SUM($C$32:$J$32)</f>
+        <v>0.85401459854014594</v>
+      </c>
+      <c r="D34" s="90"/>
+      <c r="E34" s="90"/>
+      <c r="F34" s="90"/>
+      <c r="G34" s="90">
+        <f>G32/SUM($C$32:$J$32)</f>
+        <v>0.145985401459854</v>
+      </c>
+      <c r="H34" s="90"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="59"/>
+      <c r="L34" s="60"/>
+      <c r="M34" s="61"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="B35" s="72"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="78"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="61"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="60">
+      <c r="B36" s="39"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="59"/>
+      <c r="L36" s="60">
         <f>L31</f>
         <v>54400</v>
       </c>
-      <c r="M34" s="61"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="38" t="s">
+      <c r="M36" s="98">
+        <f>L36/L38</f>
+        <v>0.65621230398069963</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="39" t="s">
+      <c r="B37" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="62"/>
-      <c r="K35" s="59"/>
-      <c r="L35" s="42">
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="62"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="42">
         <f>MIN($L$12,L30)</f>
         <v>40000</v>
       </c>
-      <c r="M35" s="61"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="38" t="s">
+      <c r="M37" s="61"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="39" t="s">
+      <c r="B38" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="69"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="42">
-        <f>MAX(L25-L35,0)</f>
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="68"/>
+      <c r="K38" s="59"/>
+      <c r="L38" s="42">
+        <f>MAX(L25-L37,0)</f>
         <v>82900</v>
       </c>
-      <c r="M36" s="61"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B37" s="39"/>
-      <c r="C37" s="84">
-        <f>L36/$L$36</f>
-        <v>1</v>
-      </c>
-      <c r="D37" s="84"/>
-      <c r="E37" s="84"/>
-      <c r="F37" s="84"/>
-      <c r="G37" s="84"/>
-      <c r="H37" s="84"/>
-      <c r="I37" s="84"/>
-      <c r="J37" s="84"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="81"/>
-      <c r="M37" s="61"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A38" s="72" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" s="73"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
-      <c r="H38" s="82"/>
-      <c r="I38" s="82"/>
-      <c r="J38" s="82"/>
-      <c r="K38" s="79"/>
-      <c r="L38" s="83"/>
       <c r="M38" s="61"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="38" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B39" s="39"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="69"/>
-      <c r="H39" s="69"/>
-      <c r="I39" s="69"/>
-      <c r="J39" s="69"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="84"/>
+      <c r="H39" s="84"/>
+      <c r="I39" s="84"/>
+      <c r="J39" s="84"/>
       <c r="K39" s="59"/>
       <c r="L39" s="42">
-        <f>L36</f>
-        <v>82900</v>
-      </c>
-      <c r="M39" s="61"/>
+        <f>L38-L36</f>
+        <v>28500</v>
+      </c>
+      <c r="M39" s="98">
+        <f>L39/L38</f>
+        <v>0.34378769601930037</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="38" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="B40" s="39"/>
-      <c r="C40" s="41">
-        <f>$C$37*$C$32*C26*$L$40</f>
+      <c r="C40" s="90">
+        <f>L38/$L$38</f>
+        <v>1</v>
+      </c>
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="90"/>
+      <c r="G40" s="90"/>
+      <c r="H40" s="90"/>
+      <c r="I40" s="90"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="59"/>
+      <c r="L40" s="80"/>
+      <c r="M40" s="61"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="71" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="72"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
+      <c r="J41" s="81"/>
+      <c r="K41" s="78"/>
+      <c r="L41" s="82"/>
+      <c r="M41" s="61"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" s="39"/>
+      <c r="C42" s="83">
+        <f>C26*(C33*$M$36+C34*$M$39)</f>
+        <v>0.84128610733362641</v>
+      </c>
+      <c r="D42" s="83">
+        <f>D26*(C33*$M$36+C34*$M$39)</f>
+        <v>8.4128610733362641E-2</v>
+      </c>
+      <c r="E42" s="83">
+        <f>E26*(C33*$M$36+C34*$M$39)</f>
+        <v>2.103215268334066E-2</v>
+      </c>
+      <c r="F42" s="83">
+        <f>F26*(C33*$M$36+C34*$M$39)</f>
+        <v>3.3651444293345055E-3</v>
+      </c>
+      <c r="G42" s="83">
+        <f>G26*(G33*$M$36+G34*$M$39)</f>
+        <v>5.0187984820335818E-2</v>
+      </c>
+      <c r="H42" s="83">
+        <f>H26*(G33*$M$36+G34*$M$39)</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="83">
+        <f>I26*(G33*$M$36+G34*$M$39)</f>
+        <v>0</v>
+      </c>
+      <c r="J42" s="83">
+        <f>J26*(G33*$M$36+G34*$M$39)</f>
+        <v>0</v>
+      </c>
+      <c r="K42" s="59"/>
+      <c r="L42" s="80"/>
+      <c r="M42" s="61"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="39"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="68"/>
+      <c r="J43" s="68"/>
+      <c r="K43" s="59"/>
+      <c r="L43" s="42">
+        <f>L38</f>
+        <v>82900</v>
+      </c>
+      <c r="M43" s="61"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" s="39"/>
+      <c r="C44" s="41">
+        <f>$C$40*$C$33*C26*$L$44</f>
         <v>44286.979627989371</v>
       </c>
-      <c r="D40" s="41">
-        <f t="shared" ref="D40:J40" si="1">$C$37*$C$32*D26*$L$40</f>
+      <c r="D44" s="41">
+        <f>$C$40*$C$33*D26*$L$44</f>
         <v>4428.6979627989376</v>
       </c>
-      <c r="E40" s="41">
+      <c r="E44" s="41">
+        <f>$C$40*$C$33*E26*$L$44</f>
+        <v>1107.1744906997344</v>
+      </c>
+      <c r="F44" s="41">
+        <f>$C$40*$C$33*F26*$L$44</f>
+        <v>177.1479185119575</v>
+      </c>
+      <c r="G44" s="41">
+        <f>$C$40*$G$33*G26*$L$44</f>
+        <v>0</v>
+      </c>
+      <c r="H44" s="41">
+        <f>$C$40*$G$33*H26*$L$44</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="41">
+        <f>$C$40*$G$33*I26*$L$44</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="41">
+        <f>$C$40*$G$33*J26*$L$44</f>
+        <v>0</v>
+      </c>
+      <c r="K44" s="59"/>
+      <c r="L44" s="42">
+        <f>MIN(MAX(L43-L15,0),L16)</f>
+        <v>50000</v>
+      </c>
+      <c r="M44" s="61"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="39"/>
+      <c r="C45" s="41">
+        <f>C42*$L$44</f>
+        <v>42064.305366681321</v>
+      </c>
+      <c r="D45" s="41">
+        <f t="shared" ref="D45:J47" si="1">D42*$L$44</f>
+        <v>4206.4305366681319</v>
+      </c>
+      <c r="E45" s="41">
         <f t="shared" si="1"/>
-        <v>1107.1744906997344</v>
-      </c>
-      <c r="F40" s="41">
+        <v>1051.607634167033</v>
+      </c>
+      <c r="F45" s="41">
         <f t="shared" si="1"/>
-        <v>177.1479185119575</v>
-      </c>
-      <c r="G40" s="41">
-        <f>$C$37*$G$32*G26*$L$40</f>
-        <v>0</v>
-      </c>
-      <c r="H40" s="41">
-        <f t="shared" ref="H40:J40" si="2">$C$37*$G$32*H26*$L$40</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="41">
+        <v>168.25722146672527</v>
+      </c>
+      <c r="G45" s="41">
+        <f t="shared" si="1"/>
+        <v>2509.3992410167907</v>
+      </c>
+      <c r="H45" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I45" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J45" s="41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="59"/>
+      <c r="L45" s="42"/>
+      <c r="M45" s="61"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="39"/>
+      <c r="C46" s="41">
+        <f>$C$40*$C$33*C26*$L$46</f>
+        <v>29140.832595217005</v>
+      </c>
+      <c r="D46" s="41">
+        <f>$C$40*$C$33*D26*$L$46</f>
+        <v>2914.0832595217007</v>
+      </c>
+      <c r="E46" s="41">
+        <f>$C$40*$C$33*E26*$L$46</f>
+        <v>728.52081488042518</v>
+      </c>
+      <c r="F46" s="41">
+        <f>$C$40*$C$33*F26*$L$46</f>
+        <v>116.56333038086802</v>
+      </c>
+      <c r="G46" s="41">
+        <f>$C$40*$G$33*G26*$L$46</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="41">
+        <f>$C$40*$G$33*H26*$L$46</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="41">
+        <f>$C$40*$G$33*I26*$L$46</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="41">
+        <f>$C$40*$G$33*J26*$L$46</f>
+        <v>0</v>
+      </c>
+      <c r="K46" s="56"/>
+      <c r="L46" s="42">
+        <f>MIN(MAX(L43-L18,0),L19)</f>
+        <v>32900</v>
+      </c>
+      <c r="M46" s="61"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="39"/>
+      <c r="C47" s="41">
+        <f>C42*$L$46</f>
+        <v>27678.312931276309</v>
+      </c>
+      <c r="D47" s="41">
+        <f t="shared" ref="D47:J47" si="2">D42*$L$46</f>
+        <v>2767.8312931276309</v>
+      </c>
+      <c r="E47" s="41">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J40" s="41">
+        <v>691.95782328190774</v>
+      </c>
+      <c r="F47" s="41">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K40" s="59"/>
-      <c r="L40" s="42">
-        <f>MIN(MAX(L39-L15,0),L16)</f>
-        <v>50000</v>
-      </c>
-      <c r="M40" s="61"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="41">
-        <f>$C$37*$C$32*C26*$L$41</f>
-        <v>29140.832595217005</v>
-      </c>
-      <c r="D41" s="41">
-        <f t="shared" ref="D41:J41" si="3">$C$37*$C$32*D26*$L$41</f>
-        <v>2914.0832595217007</v>
-      </c>
-      <c r="E41" s="41">
-        <f t="shared" si="3"/>
-        <v>728.52081488042518</v>
-      </c>
-      <c r="F41" s="41">
-        <f t="shared" si="3"/>
-        <v>116.56333038086802</v>
-      </c>
-      <c r="G41" s="41">
-        <f>$C$37*$G$32*G26*$L$41</f>
-        <v>0</v>
-      </c>
-      <c r="H41" s="41">
-        <f t="shared" ref="H41:J41" si="4">$C$37*$G$32*H26*$L$41</f>
-        <v>0</v>
-      </c>
-      <c r="I41" s="41">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J41" s="41">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K41" s="56"/>
-      <c r="L41" s="42">
-        <f>MIN(MAX(L39-L18,0),L19)</f>
-        <v>32900</v>
-      </c>
-      <c r="M41" s="61"/>
-    </row>
-    <row r="42" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="63" t="s">
+        <v>110.71325172510522</v>
+      </c>
+      <c r="G47" s="41">
+        <f t="shared" si="2"/>
+        <v>1651.1847005890484</v>
+      </c>
+      <c r="H47" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K47" s="56"/>
+      <c r="L47" s="42"/>
+      <c r="M47" s="61"/>
+    </row>
+    <row r="48" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="B42" s="51"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="64"/>
-      <c r="E42" s="64"/>
-      <c r="F42" s="64"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="64"/>
-      <c r="I42" s="64"/>
-      <c r="J42" s="64"/>
-      <c r="K42" s="65"/>
-      <c r="L42" s="66">
-        <f>SUM(C42:J42)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="67"/>
-      <c r="B44" s="67"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26"/>
-      <c r="K44" s="68"/>
-    </row>
-    <row r="45" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="39"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="39"/>
-    </row>
-    <row r="46" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="39"/>
-      <c r="B46" s="39"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="56"/>
-    </row>
-    <row r="47" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="67"/>
-      <c r="B47" s="67"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="39"/>
-    </row>
-    <row r="48" spans="1:13" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="39"/>
-      <c r="B48" s="39"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="49"/>
-      <c r="I48" s="49"/>
-      <c r="J48" s="49"/>
-      <c r="K48" s="57"/>
-    </row>
-    <row r="49" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="39"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="49"/>
-      <c r="J49" s="49"/>
-      <c r="K49" s="56"/>
-    </row>
-    <row r="50" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="39"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="39"/>
-    </row>
-    <row r="51" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="67"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="23"/>
-      <c r="I51" s="23"/>
-      <c r="J51" s="23"/>
-      <c r="K51" s="39"/>
-    </row>
-    <row r="52" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="39"/>
-      <c r="B52" s="39"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="53"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="53"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="53"/>
-      <c r="J52" s="53"/>
-      <c r="K52" s="39"/>
-    </row>
-    <row r="53" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="39"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="23"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="64"/>
+      <c r="K48" s="65"/>
+      <c r="L48" s="66">
+        <f>SUM(C48:J48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="67"/>
+    </row>
+    <row r="50" spans="1:12" s="94" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="91"/>
+      <c r="B50" s="92"/>
+      <c r="C50" s="93"/>
+      <c r="D50" s="93"/>
+      <c r="E50" s="93"/>
+      <c r="F50" s="93"/>
+      <c r="G50" s="93"/>
+      <c r="H50" s="93"/>
+      <c r="I50" s="93"/>
+      <c r="J50" s="93"/>
+      <c r="K50" s="91"/>
+      <c r="L50" s="97"/>
+    </row>
+    <row r="51" spans="1:12" s="94" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="92"/>
+      <c r="B51" s="92"/>
+      <c r="C51" s="93"/>
+      <c r="D51" s="93"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="93"/>
+      <c r="G51" s="93"/>
+      <c r="H51" s="93"/>
+      <c r="I51" s="93"/>
+      <c r="J51" s="93"/>
+      <c r="K51" s="92"/>
+      <c r="L51" s="97"/>
+    </row>
+    <row r="52" spans="1:12" s="94" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="91"/>
+      <c r="B52" s="92"/>
+      <c r="C52" s="95"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="95"/>
+      <c r="F52" s="95"/>
+      <c r="G52" s="95"/>
+      <c r="H52" s="95"/>
+      <c r="I52" s="95"/>
+      <c r="J52" s="95"/>
+      <c r="K52" s="96"/>
+      <c r="L52" s="97"/>
+    </row>
+    <row r="53" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="67"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="41"/>
       <c r="K53" s="39"/>
     </row>
-    <row r="54" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="67"/>
+    <row r="54" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="39"/>
       <c r="B54" s="39"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="39"/>
-    </row>
-    <row r="55" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="57"/>
+    </row>
+    <row r="55" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="39"/>
       <c r="B55" s="39"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="41"/>
-      <c r="H55" s="41"/>
-      <c r="I55" s="41"/>
-      <c r="J55" s="41"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
       <c r="K55" s="56"/>
     </row>
-    <row r="56" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="39"/>
       <c r="B56" s="39"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
-      <c r="H56" s="41"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="56"/>
-    </row>
-    <row r="57" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="39"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23"/>
+      <c r="K56" s="39"/>
+    </row>
+    <row r="57" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="67"/>
       <c r="B57" s="39"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="41"/>
-      <c r="H57" s="41"/>
-      <c r="I57" s="41"/>
-      <c r="J57" s="41"/>
-      <c r="K57" s="56"/>
-    </row>
-    <row r="58" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="23"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="39"/>
+    </row>
+    <row r="58" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="39"/>
       <c r="B58" s="39"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
-      <c r="E58" s="23"/>
-      <c r="F58" s="23"/>
-      <c r="G58" s="23"/>
-      <c r="H58" s="23"/>
-      <c r="I58" s="23"/>
-      <c r="J58" s="23"/>
+      <c r="C58" s="53"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="53"/>
+      <c r="H58" s="53"/>
+      <c r="I58" s="53"/>
+      <c r="J58" s="53"/>
       <c r="K58" s="39"/>
     </row>
-    <row r="59" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A60" s="45"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="45"/>
+    <row r="59" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="39"/>
+      <c r="B59" s="39"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
+      <c r="I59" s="23"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="39"/>
+    </row>
+    <row r="60" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="67"/>
+      <c r="B60" s="39"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="23"/>
+      <c r="I60" s="23"/>
+      <c r="J60" s="23"/>
+      <c r="K60" s="39"/>
+    </row>
+    <row r="61" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="39"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="41"/>
+      <c r="I61" s="41"/>
+      <c r="J61" s="41"/>
+      <c r="K61" s="56"/>
+    </row>
+    <row r="62" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="39"/>
+      <c r="B62" s="39"/>
+      <c r="C62" s="41"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="41"/>
+      <c r="I62" s="41"/>
+      <c r="J62" s="41"/>
+      <c r="K62" s="56"/>
+    </row>
+    <row r="63" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="39"/>
+      <c r="B63" s="39"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="41"/>
+      <c r="E63" s="41"/>
+      <c r="F63" s="41"/>
+      <c r="G63" s="41"/>
+      <c r="H63" s="41"/>
+      <c r="I63" s="41"/>
+      <c r="J63" s="41"/>
+      <c r="K63" s="56"/>
+    </row>
+    <row r="64" spans="1:12" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="39"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="39"/>
+    </row>
+    <row r="65" spans="1:1" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="45"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="17">
+    <mergeCell ref="C40:J40"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="G34:J34"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="G28:J28"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="G29:J29"/>
-    <mergeCell ref="C37:J37"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
@@ -3079,13 +3350,13 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="88" t="s">
+      <c r="A36" s="85" t="s">
         <v>121</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="88" t="s">
+      <c r="C36" s="85" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3581,19 +3852,19 @@
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="89" t="s">
+      <c r="A69" s="86" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A70" s="85" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A70" s="88" t="s">
+      <c r="C70" s="85" t="s">
         <v>127</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C70" s="88" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>